<commit_message>
18 08 05 antes da aula
</commit_message>
<xml_diff>
--- a/melhoras no killerbreak.xlsx
+++ b/melhoras no killerbreak.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24334"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9F5F94-C3D8-426A-BC9C-6F155EFBD141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E5009C-4F88-4598-BF42-695B4E944479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="etapas" sheetId="2" r:id="rId1"/>
@@ -686,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:R17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1280,8 +1280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEAD0173-18FD-4923-85D7-E96165695F10}">
   <dimension ref="B2:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>